<commit_message>
at bracken co with LNA data file transfers/hunt/seek
</commit_message>
<xml_diff>
--- a/dat/select2cols.xlsx
+++ b/dat/select2cols.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="81">
   <si>
     <t xml:space="preserve">FID</t>
   </si>
@@ -31,9 +31,15 @@
     <t xml:space="preserve">Listing</t>
   </si>
   <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
     <t xml:space="preserve">Allen County</t>
   </si>
   <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Anderson County</t>
   </si>
   <si>
@@ -47,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">Bourbon County</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
   </si>
   <si>
     <t xml:space="preserve">Boyd County</t>
@@ -268,6 +277,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -349,18 +359,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E52" activeCellId="0" sqref="E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="156.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="64.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -373,6 +383,9 @@
       <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -382,12 +395,15 @@
         <v>41</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" s="0" t="str">
         <f aca="false">LEFT(C2, FIND(" ", C2)-1)</f>
         <v>Allen</v>
       </c>
+      <c r="E2" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -397,12 +413,15 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D3" s="0" t="str">
         <f aca="false">LEFT(C3, FIND(" ", C3)-1)</f>
         <v>Anderson</v>
       </c>
+      <c r="E3" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -412,10 +431,13 @@
         <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -426,12 +448,15 @@
         <v>10</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D5" s="0" t="str">
         <f aca="false">LEFT(C5, FIND(" ", C5)-1)</f>
         <v>Bell</v>
       </c>
+      <c r="E5" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -441,12 +466,15 @@
         <v>37</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D6" s="0" t="str">
         <f aca="false">LEFT(C6, FIND(" ", C6)-1)</f>
         <v>Bourbon</v>
       </c>
+      <c r="E6" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -456,12 +484,15 @@
         <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D7" s="0" t="str">
         <f aca="false">LEFT(C7, FIND(" ", C7)-1)</f>
         <v>Boyd</v>
       </c>
+      <c r="E7" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -471,12 +502,15 @@
         <v>58</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D8" s="0" t="str">
         <f aca="false">LEFT(C8, FIND(" ", C8)-1)</f>
         <v>Boyle</v>
       </c>
+      <c r="E8" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -486,12 +520,15 @@
         <v>60</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D9" s="0" t="str">
         <f aca="false">LEFT(C9, FIND(" ", C9)-1)</f>
         <v>Bracken</v>
       </c>
+      <c r="E9" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -501,12 +538,15 @@
         <v>55</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D10" s="0" t="str">
         <f aca="false">LEFT(C10, FIND(" ", C10)-1)</f>
         <v>Breathitt</v>
       </c>
+      <c r="E10" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -516,12 +556,15 @@
         <v>57</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D11" s="0" t="str">
         <f aca="false">LEFT(C11, FIND(" ", C11)-1)</f>
         <v>Breckinridge</v>
       </c>
+      <c r="E11" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -531,10 +574,13 @@
         <v>39</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -545,12 +591,15 @@
         <v>45</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D13" s="0" t="str">
         <f aca="false">LEFT(C13, FIND(" ", C13)-1)</f>
         <v>Bullitt</v>
       </c>
+      <c r="E13" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -560,12 +609,15 @@
         <v>5</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D14" s="0" t="str">
         <f aca="false">LEFT(C14, FIND(" ", C14)-1)</f>
         <v>Calloway</v>
       </c>
+      <c r="E14" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -575,12 +627,15 @@
         <v>40</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D15" s="0" t="str">
         <f aca="false">LEFT(C15, FIND(" ", C15)-1)</f>
         <v>Carter</v>
       </c>
+      <c r="E15" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -590,12 +645,15 @@
         <v>56</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D16" s="0" t="str">
         <f aca="false">LEFT(C16, FIND(" ", C16)-1)</f>
         <v>Christian</v>
       </c>
+      <c r="E16" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -605,12 +663,15 @@
         <v>43</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D17" s="0" t="str">
         <f aca="false">LEFT(C17, FIND(" ", C17)-1)</f>
         <v>Clark</v>
       </c>
+      <c r="E17" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -620,10 +681,13 @@
         <v>19</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -634,12 +698,15 @@
         <v>46</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D19" s="0" t="str">
         <f aca="false">LEFT(C19, FIND(" ", C19)-1)</f>
         <v>Estill</v>
       </c>
+      <c r="E19" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -649,12 +716,15 @@
         <v>49</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D20" s="0" t="str">
         <f aca="false">LEFT(C20, FIND(" ", C20)-1)</f>
         <v>Fayette</v>
       </c>
+      <c r="E20" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -664,12 +734,15 @@
         <v>50</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D21" s="0" t="str">
         <f aca="false">LEFT(C21, FIND(" ", C21)-1)</f>
         <v>Fleming</v>
       </c>
+      <c r="E21" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -679,12 +752,15 @@
         <v>3</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D22" s="0" t="str">
         <f aca="false">LEFT(C22, FIND(" ", C22)-1)</f>
         <v>Floyd</v>
       </c>
+      <c r="E22" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -694,12 +770,15 @@
         <v>18</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D23" s="0" t="str">
         <f aca="false">LEFT(C23, FIND(" ", C23)-1)</f>
         <v>Franklin</v>
       </c>
+      <c r="E23" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -709,12 +788,15 @@
         <v>27</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D24" s="0" t="str">
         <f aca="false">LEFT(C24, FIND(" ", C24)-1)</f>
         <v>Garrard</v>
       </c>
+      <c r="E24" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -724,10 +806,13 @@
         <v>16</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -738,12 +823,15 @@
         <v>44</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D26" s="0" t="str">
         <f aca="false">LEFT(C26, FIND(" ", C26)-1)</f>
         <v>Graves</v>
       </c>
+      <c r="E26" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -753,12 +841,15 @@
         <v>36</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D27" s="0" t="str">
         <f aca="false">LEFT(C27, FIND(" ", C27)-1)</f>
         <v>Grayson</v>
       </c>
+      <c r="E27" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -768,10 +859,13 @@
         <v>15</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -782,12 +876,15 @@
         <v>33</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D29" s="0" t="str">
         <f aca="false">LEFT(C29, FIND(" ", C29)-1)</f>
         <v>Greenup</v>
       </c>
+      <c r="E29" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -797,12 +894,15 @@
         <v>22</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D30" s="0" t="str">
         <f aca="false">LEFT(C30, FIND(" ", C30)-1)</f>
         <v>Harlan</v>
       </c>
+      <c r="E30" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -812,12 +912,15 @@
         <v>6</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D31" s="0" t="str">
         <f aca="false">LEFT(C31, FIND(" ", C31)-1)</f>
         <v>Hopkins</v>
       </c>
+      <c r="E31" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -827,12 +930,15 @@
         <v>12</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D32" s="0" t="str">
         <f aca="false">LEFT(C32, FIND(" ", C32)-1)</f>
         <v>Jefferson</v>
       </c>
+      <c r="E32" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -842,12 +948,15 @@
         <v>59</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D33" s="0" t="str">
         <f aca="false">LEFT(C33, FIND(" ", C33)-1)</f>
         <v>Jessamine</v>
       </c>
+      <c r="E33" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -857,12 +966,15 @@
         <v>32</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D34" s="0" t="str">
         <f aca="false">LEFT(C34, FIND(" ", C34)-1)</f>
         <v>Johnson</v>
       </c>
+      <c r="E34" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -872,10 +984,13 @@
         <v>20</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -886,12 +1001,15 @@
         <v>2</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D36" s="0" t="str">
         <f aca="false">LEFT(C36, FIND(" ", C36)-1)</f>
         <v>Knox</v>
       </c>
+      <c r="E36" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
@@ -901,10 +1019,13 @@
         <v>1</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -915,12 +1036,15 @@
         <v>4</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D38" s="0" t="str">
         <f aca="false">LEFT(C38, FIND(" ", C38)-1)</f>
         <v>Laurel</v>
       </c>
+      <c r="E38" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
@@ -930,12 +1054,15 @@
         <v>29</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D39" s="0" t="str">
         <f aca="false">LEFT(C39, FIND(" ", C39)-1)</f>
         <v>Lawrence</v>
       </c>
+      <c r="E39" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
@@ -945,12 +1072,15 @@
         <v>25</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D40" s="0" t="str">
         <f aca="false">LEFT(C40, FIND(" ", C40)-1)</f>
         <v>Lewis</v>
       </c>
+      <c r="E40" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
@@ -960,12 +1090,15 @@
         <v>11</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D41" s="0" t="str">
         <f aca="false">LEFT(C41, FIND(" ", C41)-1)</f>
         <v>Lincoln</v>
       </c>
+      <c r="E41" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
@@ -975,10 +1108,13 @@
         <v>35</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -989,12 +1125,15 @@
         <v>34</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D43" s="0" t="str">
         <f aca="false">LEFT(C43, FIND(" ", C43)-1)</f>
         <v>Madison</v>
       </c>
+      <c r="E43" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -1004,12 +1143,15 @@
         <v>31</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D44" s="0" t="str">
         <f aca="false">LEFT(C44, FIND(" ", C44)-1)</f>
         <v>Magoffin</v>
       </c>
+      <c r="E44" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
@@ -1019,12 +1161,15 @@
         <v>21</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D45" s="0" t="str">
         <f aca="false">LEFT(C45, FIND(" ", C45)-1)</f>
         <v>Marshall</v>
       </c>
+      <c r="E45" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
@@ -1034,12 +1179,15 @@
         <v>61</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D46" s="0" t="str">
         <f aca="false">LEFT(C46, FIND(" ", C46)-1)</f>
         <v>Martin</v>
       </c>
+      <c r="E46" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
@@ -1049,12 +1197,15 @@
         <v>47</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D47" s="0" t="str">
         <f aca="false">LEFT(C47, FIND(" ", C47)-1)</f>
         <v>Mercer</v>
       </c>
+      <c r="E47" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
@@ -1064,12 +1215,15 @@
         <v>23</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D48" s="0" t="str">
         <f aca="false">LEFT(C48, FIND(" ", C48)-1)</f>
         <v>Monroe</v>
       </c>
+      <c r="E48" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
@@ -1079,12 +1233,15 @@
         <v>38</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D49" s="0" t="str">
         <f aca="false">LEFT(C49, FIND(" ", C49)-1)</f>
         <v>Montgomery</v>
       </c>
+      <c r="E49" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
@@ -1094,12 +1251,15 @@
         <v>48</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D50" s="0" t="str">
         <f aca="false">LEFT(C50, FIND(" ", C50)-1)</f>
         <v>Muhlenberg</v>
       </c>
+      <c r="E50" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
@@ -1109,10 +1269,13 @@
         <v>9</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1123,10 +1286,13 @@
         <v>13</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1137,12 +1303,15 @@
         <v>30</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D53" s="0" t="str">
         <f aca="false">LEFT(C53, FIND(" ", C53)-1)</f>
         <v>Oldham</v>
       </c>
+      <c r="E53" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
@@ -1152,10 +1321,13 @@
         <v>26</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1166,12 +1338,15 @@
         <v>53</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D55" s="0" t="str">
         <f aca="false">LEFT(C55, FIND(" ", C55)-1)</f>
         <v>Pike</v>
       </c>
+      <c r="E55" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
@@ -1181,12 +1356,15 @@
         <v>54</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D56" s="0" t="str">
         <f aca="false">LEFT(C56, FIND(" ", C56)-1)</f>
         <v>Powell</v>
       </c>
+      <c r="E56" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
@@ -1196,10 +1374,13 @@
         <v>28</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1210,10 +1391,13 @@
         <v>24</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1224,12 +1408,15 @@
         <v>42</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D59" s="0" t="str">
         <f aca="false">LEFT(C59, FIND(" ", C59)-1)</f>
         <v>Todd</v>
       </c>
+      <c r="E59" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
@@ -1239,10 +1426,13 @@
         <v>8</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1253,12 +1443,15 @@
         <v>51</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D61" s="0" t="str">
         <f aca="false">LEFT(C61, FIND(" ", C61)-1)</f>
         <v>Whitley</v>
       </c>
+      <c r="E61" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
@@ -1268,11 +1461,14 @@
         <v>52</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D62" s="0" t="str">
         <f aca="false">LEFT(C62, FIND(" ", C62)-1)</f>
         <v>Woodford</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>